<commit_message>
Feina de avui 10/06/2015
</commit_message>
<xml_diff>
--- a/app/src/main/res/externs/analisi/Definicions Android.xlsx
+++ b/app/src/main/res/externs/analisi/Definicions Android.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="77">
   <si>
     <t>Component</t>
   </si>
@@ -543,6 +543,42 @@
   </si>
   <si>
     <t>nom layoutMNUnom (si menú)</t>
+  </si>
+  <si>
+    <t>Objecte</t>
+  </si>
+  <si>
+    <t>Edit text</t>
+  </si>
+  <si>
+    <t>ETX</t>
+  </si>
+  <si>
+    <t>TXT</t>
+  </si>
+  <si>
+    <t>Text field (literal)</t>
+  </si>
+  <si>
+    <t>SPN</t>
+  </si>
+  <si>
+    <t>Request Code</t>
+  </si>
+  <si>
+    <t>RQC</t>
+  </si>
+  <si>
+    <t>Strings de BBDD</t>
+  </si>
+  <si>
+    <t>R.string.TNom taula_nom</t>
+  </si>
+  <si>
+    <t>ListView</t>
+  </si>
+  <si>
+    <t>LVW</t>
   </si>
 </sst>
 </file>
@@ -609,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -623,6 +659,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -924,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,65 +1040,69 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-    </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
@@ -1075,125 +1116,125 @@
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-    </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
+      <c r="A36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -1203,49 +1244,45 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
@@ -1255,9 +1292,89 @@
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
+    <row r="46" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>